<commit_message>
Adventures of Batman and Robin
</commit_message>
<xml_diff>
--- a/Лист Microsoft Excel.xlsx
+++ b/Лист Microsoft Excel.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Z" sheetId="1" r:id="rId1"/>
     <sheet name="Y" sheetId="2" r:id="rId2"/>
     <sheet name="X" sheetId="3" r:id="rId3"/>
+    <sheet name="#" sheetId="4" r:id="rId4"/>
+    <sheet name="A" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="117">
   <si>
     <t>Zan: Yasha Enbukyoku</t>
   </si>
@@ -132,6 +134,246 @@
   </si>
   <si>
     <t>Xump 2: Back in Space</t>
+  </si>
+  <si>
+    <t>007 Shitou</t>
+  </si>
+  <si>
+    <t>10 Super Jogos</t>
+  </si>
+  <si>
+    <t>16 Tiles Mahjong</t>
+  </si>
+  <si>
+    <t>16Bit Rhythm Land</t>
+  </si>
+  <si>
+    <t>16t</t>
+  </si>
+  <si>
+    <t>1985 World Cup</t>
+  </si>
+  <si>
+    <t>2020 Nen Super Baseball</t>
+  </si>
+  <si>
+    <t>3 Ninjas Kick Back</t>
+  </si>
+  <si>
+    <t>30 Years of Nintendon't</t>
+  </si>
+  <si>
+    <t>6-Pak</t>
+  </si>
+  <si>
+    <t>688 Attack Sub</t>
+  </si>
+  <si>
+    <t>A-Ressha de Ikou MD</t>
+  </si>
+  <si>
+    <t>A(...)M(...)96</t>
+  </si>
+  <si>
+    <t>Aa Harimanada</t>
+  </si>
+  <si>
+    <t>AAAHH!!! Real Monsters</t>
+  </si>
+  <si>
+    <t>ACME All Stars</t>
+  </si>
+  <si>
+    <t>Action 52</t>
+  </si>
+  <si>
+    <t>Addams Family Values</t>
+  </si>
+  <si>
+    <t>Addams Family, The</t>
+  </si>
+  <si>
+    <t>Advanced Busterhawk Gley Lancer</t>
+  </si>
+  <si>
+    <t>Advanced Busterhawk Gleylancer</t>
+  </si>
+  <si>
+    <t>Advanced Daisenryaku: Deutsch Dengeki Sakusen</t>
+  </si>
+  <si>
+    <t>Adventures of Batman &amp; Robin, The</t>
+  </si>
+  <si>
+    <t>Adventures of Mighty Max, The</t>
+  </si>
+  <si>
+    <t>Adventures of Rocky and Bullwinkle and Friends, The</t>
+  </si>
+  <si>
+    <t>Aero Blasters</t>
+  </si>
+  <si>
+    <t>Aero the Acro-Bat</t>
+  </si>
+  <si>
+    <t>Aero the Acro-Bat 2</t>
+  </si>
+  <si>
+    <t>Aerobiz</t>
+  </si>
+  <si>
+    <t>Aerobiz Supersonic</t>
+  </si>
+  <si>
+    <t>After Burner II</t>
+  </si>
+  <si>
+    <t>Ageo Nara</t>
+  </si>
+  <si>
+    <t>Air Buster</t>
+  </si>
+  <si>
+    <t>Air Diver</t>
+  </si>
+  <si>
+    <t>Air Management II: Koukuu-Ou o Mezase</t>
+  </si>
+  <si>
+    <t>Air Management: Oozora ni Kakeru</t>
+  </si>
+  <si>
+    <t>Akira</t>
+  </si>
+  <si>
+    <t>Al Michaels Announces HardBall III</t>
+  </si>
+  <si>
+    <t>Alex Kidd Cheongong Maseong</t>
+  </si>
+  <si>
+    <t>Alex Kidd in the Enchanted Castle</t>
+  </si>
+  <si>
+    <t>Alex Kidd: Tenkuu Majou</t>
+  </si>
+  <si>
+    <t>Alice Sisters</t>
+  </si>
+  <si>
+    <t>Alien 3</t>
+  </si>
+  <si>
+    <t>Alien Cat 2</t>
+  </si>
+  <si>
+    <t>Alien Soldier</t>
+  </si>
+  <si>
+    <t>Alien Storm</t>
+  </si>
+  <si>
+    <t>Alisia Dragoon</t>
+  </si>
+  <si>
+    <t>Altered Beast</t>
+  </si>
+  <si>
+    <t>American Gladiators</t>
+  </si>
+  <si>
+    <t>Andre Agassi Tennis</t>
+  </si>
+  <si>
+    <t>Animaniacs</t>
+  </si>
+  <si>
+    <t>Another World</t>
+  </si>
+  <si>
+    <t>Aoki Ookami to Shiroki Mejika: Genchou Hishi</t>
+  </si>
+  <si>
+    <t>Aquatic Games estrelando James Pond e the Aquabats, The</t>
+  </si>
+  <si>
+    <t>Aquatic Games starring James Pond and the Aquabats, The</t>
+  </si>
+  <si>
+    <t>Arang Jeonseol</t>
+  </si>
+  <si>
+    <t>Arcade Classics</t>
+  </si>
+  <si>
+    <t>Arch Rivals: The Arcade Game</t>
+  </si>
+  <si>
+    <t>Arcus Odyssey</t>
+  </si>
+  <si>
+    <t>Ariel The Little Mermaid</t>
+  </si>
+  <si>
+    <t>Arkagis Revolution</t>
+  </si>
+  <si>
+    <t>Arnold Palmer Tournament Golf</t>
+  </si>
+  <si>
+    <t>Arrow Flash</t>
+  </si>
+  <si>
+    <t>Art Alive</t>
+  </si>
+  <si>
+    <t>Art of Fighting</t>
+  </si>
+  <si>
+    <t>ASCII Wars: Limited Edition</t>
+  </si>
+  <si>
+    <t>Assault Suit Leynos</t>
+  </si>
+  <si>
+    <t>Astebros</t>
+  </si>
+  <si>
+    <t>Asterix and the Great Rescue</t>
+  </si>
+  <si>
+    <t>Asterix and the Power of the Gods</t>
+  </si>
+  <si>
+    <t>Astropede</t>
+  </si>
+  <si>
+    <t>Atomic Robo-Kid</t>
+  </si>
+  <si>
+    <t>Atomic Runner</t>
+  </si>
+  <si>
+    <t>ATP Tour</t>
+  </si>
+  <si>
+    <t>ATP Tour Championship Tennis</t>
+  </si>
+  <si>
+    <t>Attack of the PETSCII Robots</t>
+  </si>
+  <si>
+    <t>Australian Rugby League</t>
+  </si>
+  <si>
+    <t>Awesome Possum</t>
+  </si>
+  <si>
+    <t>Aworg</t>
+  </si>
+  <si>
+    <t>Ayrton Senna's Super Monaco GP II</t>
   </si>
 </sst>
 </file>
@@ -743,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
@@ -863,4 +1105,816 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://gamefaqs.gamespot.com/genesis/586248-james-bond-007-the-duel"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://gamefaqs.gamespot.com/genesis/620431-10-super-jogos"/>
+    <hyperlink ref="B2" r:id="rId3" display="https://gamefaqs.gamespot.com/genesis/620431-10-super-jogos/cheats"/>
+    <hyperlink ref="A3" r:id="rId4" display="https://gamefaqs.gamespot.com/genesis/621361-16-tiles-mahjong"/>
+    <hyperlink ref="B3" r:id="rId5" display="https://gamefaqs.gamespot.com/genesis/621361-16-tiles-mahjong/cheats"/>
+    <hyperlink ref="A4" r:id="rId6" display="https://gamefaqs.gamespot.com/genesis/303743-16bit-rhythm-land"/>
+    <hyperlink ref="A5" r:id="rId7" display="https://gamefaqs.gamespot.com/genesis/951912-16t"/>
+    <hyperlink ref="A6" r:id="rId8" display="https://gamefaqs.gamespot.com/genesis/437915-1985-world-cup"/>
+    <hyperlink ref="A7" r:id="rId9" display="https://gamefaqs.gamespot.com/genesis/586501-super-baseball-2020"/>
+    <hyperlink ref="A8" r:id="rId10" display="https://gamefaqs.gamespot.com/genesis/586003-3-ninjas-kick-back"/>
+    <hyperlink ref="B8" r:id="rId11" display="https://gamefaqs.gamespot.com/genesis/586003-3-ninjas-kick-back/cheats"/>
+    <hyperlink ref="A9" r:id="rId12" display="https://gamefaqs.gamespot.com/genesis/358193-30-years-of-nintendont"/>
+    <hyperlink ref="A10" r:id="rId13" display="https://gamefaqs.gamespot.com/genesis/579589-6-pak"/>
+    <hyperlink ref="B10" r:id="rId14" display="https://gamefaqs.gamespot.com/genesis/579589-6-pak/cheats"/>
+    <hyperlink ref="A11" r:id="rId15" display="https://gamefaqs.gamespot.com/genesis/586004-688-attack-sub"/>
+    <hyperlink ref="B11" r:id="rId16" display="https://gamefaqs.gamespot.com/genesis/586004-688-attack-sub/cheats"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId17"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A69" sqref="A1:A69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://gamefaqs.gamespot.com/genesis/570432-a-ressha-de-ikou-md"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://gamefaqs.gamespot.com/genesis/312648-am96"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://gamefaqs.gamespot.com/genesis/570458-aa-harimanada"/>
+    <hyperlink ref="B3" r:id="rId4" display="https://gamefaqs.gamespot.com/genesis/570458-aa-harimanada/cheats"/>
+    <hyperlink ref="A4" r:id="rId5" display="https://gamefaqs.gamespot.com/genesis/586014-aaahh-real-monsters"/>
+    <hyperlink ref="B4" r:id="rId6" display="https://gamefaqs.gamespot.com/genesis/586014-aaahh-real-monsters/cheats"/>
+    <hyperlink ref="A5" r:id="rId7" display="https://gamefaqs.gamespot.com/genesis/586542-tiny-toon-adventures-acme-all-stars"/>
+    <hyperlink ref="B5" r:id="rId8" display="https://gamefaqs.gamespot.com/genesis/586542-tiny-toon-adventures-acme-all-stars/cheats"/>
+    <hyperlink ref="A6" r:id="rId9" display="https://gamefaqs.gamespot.com/genesis/915587-action-52"/>
+    <hyperlink ref="A7" r:id="rId10" display="https://gamefaqs.gamespot.com/genesis/586007-addams-family-values"/>
+    <hyperlink ref="A8" r:id="rId11" display="https://gamefaqs.gamespot.com/genesis/586006-the-addams-family"/>
+    <hyperlink ref="B8" r:id="rId12" display="https://gamefaqs.gamespot.com/genesis/586006-the-addams-family/cheats"/>
+    <hyperlink ref="A9" r:id="rId13" display="https://gamefaqs.gamespot.com/genesis/578841-gley-lancer"/>
+    <hyperlink ref="B9" r:id="rId14" display="https://gamefaqs.gamespot.com/genesis/578841-gley-lancer/cheats"/>
+    <hyperlink ref="A10" r:id="rId15" display="https://gamefaqs.gamespot.com/genesis/578841-gley-lancer"/>
+    <hyperlink ref="B10" r:id="rId16" display="https://gamefaqs.gamespot.com/genesis/578841-gley-lancer/cheats"/>
+    <hyperlink ref="A11" r:id="rId17" display="https://gamefaqs.gamespot.com/genesis/569352-advanced-daisenryaku-deutsch-dengeki-sakusen"/>
+    <hyperlink ref="B11" r:id="rId18" display="https://gamefaqs.gamespot.com/genesis/569352-advanced-daisenryaku-deutsch-dengeki-sakusen/cheats"/>
+    <hyperlink ref="A12" r:id="rId19" display="https://gamefaqs.gamespot.com/genesis/586008-the-adventures-of-batman-and-robin"/>
+    <hyperlink ref="B12" r:id="rId20" display="https://gamefaqs.gamespot.com/genesis/586008-the-adventures-of-batman-and-robin/cheats"/>
+    <hyperlink ref="A13" r:id="rId21" display="https://gamefaqs.gamespot.com/genesis/586009-the-adventures-of-mighty-max"/>
+    <hyperlink ref="B13" r:id="rId22" display="https://gamefaqs.gamespot.com/genesis/586009-the-adventures-of-mighty-max/cheats"/>
+    <hyperlink ref="A14" r:id="rId23" display="https://gamefaqs.gamespot.com/genesis/586431-the-adventures-of-rocky-and-bullwinkle-and-friends"/>
+    <hyperlink ref="A15" r:id="rId24" display="https://gamefaqs.gamespot.com/genesis/932939-air-buster"/>
+    <hyperlink ref="A16" r:id="rId25" display="https://gamefaqs.gamespot.com/genesis/586010-aero-the-acro-bat"/>
+    <hyperlink ref="B16" r:id="rId26" display="https://gamefaqs.gamespot.com/genesis/586010-aero-the-acro-bat/cheats"/>
+    <hyperlink ref="A17" r:id="rId27" display="https://gamefaqs.gamespot.com/genesis/586011-aero-the-acro-bat-2"/>
+    <hyperlink ref="B17" r:id="rId28" display="https://gamefaqs.gamespot.com/genesis/586011-aero-the-acro-bat-2/cheats"/>
+    <hyperlink ref="A18" r:id="rId29" display="https://gamefaqs.gamespot.com/genesis/586012-aerobiz"/>
+    <hyperlink ref="A19" r:id="rId30" display="https://gamefaqs.gamespot.com/genesis/586013-aerobiz-supersonic"/>
+    <hyperlink ref="A20" r:id="rId31" display="https://gamefaqs.gamespot.com/genesis/563310-after-burner-ii"/>
+    <hyperlink ref="B20" r:id="rId32" display="https://gamefaqs.gamespot.com/genesis/563310-after-burner-ii/cheats"/>
+    <hyperlink ref="A21" r:id="rId33" display="https://gamefaqs.gamespot.com/genesis/570391-wani-wani-world"/>
+    <hyperlink ref="B21" r:id="rId34" display="https://gamefaqs.gamespot.com/genesis/570391-wani-wani-world/cheats"/>
+    <hyperlink ref="A22" r:id="rId35" display="https://gamefaqs.gamespot.com/genesis/932939-air-buster"/>
+    <hyperlink ref="A23" r:id="rId36" display="https://gamefaqs.gamespot.com/genesis/586015-air-diver"/>
+    <hyperlink ref="B23" r:id="rId37" display="https://gamefaqs.gamespot.com/genesis/586015-air-diver/cheats"/>
+    <hyperlink ref="A24" r:id="rId38" display="https://gamefaqs.gamespot.com/genesis/586013-aerobiz-supersonic"/>
+    <hyperlink ref="A25" r:id="rId39" display="https://gamefaqs.gamespot.com/genesis/586012-aerobiz"/>
+    <hyperlink ref="A26" r:id="rId40" display="https://gamefaqs.gamespot.com/genesis/280786-akira-cancelled"/>
+    <hyperlink ref="A27" r:id="rId41" display="https://gamefaqs.gamespot.com/genesis/586227-al-michaels-announces-hardball-iii"/>
+    <hyperlink ref="A28" r:id="rId42" display="https://gamefaqs.gamespot.com/genesis/586018-alex-kidd-in-the-enchanted-castle"/>
+    <hyperlink ref="B28" r:id="rId43" display="https://gamefaqs.gamespot.com/genesis/586018-alex-kidd-in-the-enchanted-castle/cheats"/>
+    <hyperlink ref="A29" r:id="rId44" display="https://gamefaqs.gamespot.com/genesis/586018-alex-kidd-in-the-enchanted-castle"/>
+    <hyperlink ref="B29" r:id="rId45" display="https://gamefaqs.gamespot.com/genesis/586018-alex-kidd-in-the-enchanted-castle/cheats"/>
+    <hyperlink ref="A30" r:id="rId46" display="https://gamefaqs.gamespot.com/genesis/586018-alex-kidd-in-the-enchanted-castle"/>
+    <hyperlink ref="B30" r:id="rId47" display="https://gamefaqs.gamespot.com/genesis/586018-alex-kidd-in-the-enchanted-castle/cheats"/>
+    <hyperlink ref="A31" r:id="rId48" display="https://gamefaqs.gamespot.com/genesis/411666-alice-sisters"/>
+    <hyperlink ref="B31" r:id="rId49" display="https://gamefaqs.gamespot.com/genesis/411666-alice-sisters/cheats"/>
+    <hyperlink ref="A32" r:id="rId50" display="https://gamefaqs.gamespot.com/genesis/586019-alien-3"/>
+    <hyperlink ref="B32" r:id="rId51" display="https://gamefaqs.gamespot.com/genesis/586019-alien-3/cheats"/>
+    <hyperlink ref="A33" r:id="rId52" display="https://gamefaqs.gamespot.com/genesis/358192-alien-cat-2"/>
+    <hyperlink ref="A34" r:id="rId53" display="https://gamefaqs.gamespot.com/genesis/564342-alien-soldier"/>
+    <hyperlink ref="B34" r:id="rId54" display="https://gamefaqs.gamespot.com/genesis/564342-alien-soldier/cheats"/>
+    <hyperlink ref="A35" r:id="rId55" display="https://gamefaqs.gamespot.com/genesis/586020-alien-storm"/>
+    <hyperlink ref="B35" r:id="rId56" display="https://gamefaqs.gamespot.com/genesis/586020-alien-storm/cheats"/>
+    <hyperlink ref="A36" r:id="rId57" display="https://gamefaqs.gamespot.com/genesis/586021-alisia-dragoon"/>
+    <hyperlink ref="B36" r:id="rId58" display="https://gamefaqs.gamespot.com/genesis/586021-alisia-dragoon/cheats"/>
+    <hyperlink ref="A37" r:id="rId59" display="https://gamefaqs.gamespot.com/genesis/586022-altered-beast"/>
+    <hyperlink ref="B37" r:id="rId60" display="https://gamefaqs.gamespot.com/genesis/586022-altered-beast/cheats"/>
+    <hyperlink ref="A38" r:id="rId61" display="https://gamefaqs.gamespot.com/genesis/586024-american-gladiators"/>
+    <hyperlink ref="A39" r:id="rId62" display="https://gamefaqs.gamespot.com/genesis/563311-andre-agassi-tennis"/>
+    <hyperlink ref="B39" r:id="rId63" display="https://gamefaqs.gamespot.com/genesis/563311-andre-agassi-tennis/cheats"/>
+    <hyperlink ref="A40" r:id="rId64" display="https://gamefaqs.gamespot.com/genesis/586025-animaniacs"/>
+    <hyperlink ref="B40" r:id="rId65" display="https://gamefaqs.gamespot.com/genesis/586025-animaniacs/cheats"/>
+    <hyperlink ref="A41" r:id="rId66" display="https://gamefaqs.gamespot.com/genesis/586360-out-of-this-world"/>
+    <hyperlink ref="B41" r:id="rId67" display="https://gamefaqs.gamespot.com/genesis/586360-out-of-this-world/cheats"/>
+    <hyperlink ref="A42" r:id="rId68" display="https://gamefaqs.gamespot.com/genesis/570471-genghis-khan-ii-clan-of-the-gray-wolf"/>
+    <hyperlink ref="A43" r:id="rId69" display="https://gamefaqs.gamespot.com/genesis/586026-the-aquatic-games-starring-james-pond-and-the-aquabats"/>
+    <hyperlink ref="B43" r:id="rId70" display="https://gamefaqs.gamespot.com/genesis/586026-the-aquatic-games-starring-james-pond-and-the-aquabats/cheats"/>
+    <hyperlink ref="A44" r:id="rId71" display="https://gamefaqs.gamespot.com/genesis/586026-the-aquatic-games-starring-james-pond-and-the-aquabats"/>
+    <hyperlink ref="B44" r:id="rId72" display="https://gamefaqs.gamespot.com/genesis/586026-the-aquatic-games-starring-james-pond-and-the-aquabats/cheats"/>
+    <hyperlink ref="A45" r:id="rId73" display="https://gamefaqs.gamespot.com/genesis/586176-fatal-fury"/>
+    <hyperlink ref="B45" r:id="rId74" display="https://gamefaqs.gamespot.com/genesis/586176-fatal-fury/cheats"/>
+    <hyperlink ref="A46" r:id="rId75" display="https://gamefaqs.gamespot.com/genesis/586027-arcade-classics"/>
+    <hyperlink ref="A47" r:id="rId76" display="https://gamefaqs.gamespot.com/genesis/586029-arch-rivals-the-arcade-game"/>
+    <hyperlink ref="B47" r:id="rId77" display="https://gamefaqs.gamespot.com/genesis/586029-arch-rivals-the-arcade-game/cheats"/>
+    <hyperlink ref="A48" r:id="rId78" display="https://gamefaqs.gamespot.com/genesis/586030-arcus-odyssey"/>
+    <hyperlink ref="B48" r:id="rId79" display="https://gamefaqs.gamespot.com/genesis/586030-arcus-odyssey/cheats"/>
+    <hyperlink ref="A49" r:id="rId80" display="https://gamefaqs.gamespot.com/genesis/586292-disneys-ariel-the-little-mermaid"/>
+    <hyperlink ref="B49" r:id="rId81" display="https://gamefaqs.gamespot.com/genesis/586292-disneys-ariel-the-little-mermaid/cheats"/>
+    <hyperlink ref="A50" r:id="rId82" display="https://gamefaqs.gamespot.com/genesis/310367-arkagis-revolution"/>
+    <hyperlink ref="B50" r:id="rId83" display="https://gamefaqs.gamespot.com/genesis/310367-arkagis-revolution/cheats"/>
+    <hyperlink ref="A51" r:id="rId84" display="https://gamefaqs.gamespot.com/genesis/586031-arnold-palmer-tournament-golf"/>
+    <hyperlink ref="B51" r:id="rId85" display="https://gamefaqs.gamespot.com/genesis/586031-arnold-palmer-tournament-golf/cheats"/>
+    <hyperlink ref="A52" r:id="rId86" display="https://gamefaqs.gamespot.com/genesis/586032-arrow-flash"/>
+    <hyperlink ref="B52" r:id="rId87" display="https://gamefaqs.gamespot.com/genesis/586032-arrow-flash/cheats"/>
+    <hyperlink ref="A53" r:id="rId88" display="https://gamefaqs.gamespot.com/genesis/586033-art-alive"/>
+    <hyperlink ref="B53" r:id="rId89" display="https://gamefaqs.gamespot.com/genesis/586033-art-alive/cheats"/>
+    <hyperlink ref="A54" r:id="rId90" display="https://gamefaqs.gamespot.com/genesis/563312-art-of-fighting"/>
+    <hyperlink ref="B54" r:id="rId91" display="https://gamefaqs.gamespot.com/genesis/563312-art-of-fighting/cheats"/>
+    <hyperlink ref="A55" r:id="rId92" display="https://gamefaqs.gamespot.com/genesis/357544-ascii-wars-limited-edition"/>
+    <hyperlink ref="A56" r:id="rId93" display="https://gamefaqs.gamespot.com/genesis/586520-target-earth"/>
+    <hyperlink ref="B56" r:id="rId94" display="https://gamefaqs.gamespot.com/genesis/586520-target-earth/cheats"/>
+    <hyperlink ref="A57" r:id="rId95" display="https://gamefaqs.gamespot.com/genesis/408688-astebros"/>
+    <hyperlink ref="A58" r:id="rId96" display="https://gamefaqs.gamespot.com/genesis/586034-asterix-and-the-great-rescue"/>
+    <hyperlink ref="B58" r:id="rId97" display="https://gamefaqs.gamespot.com/genesis/586034-asterix-and-the-great-rescue/cheats"/>
+    <hyperlink ref="A59" r:id="rId98" display="https://gamefaqs.gamespot.com/genesis/568093-asterix-and-the-power-of-the-gods"/>
+    <hyperlink ref="A60" r:id="rId99" display="https://gamefaqs.gamespot.com/genesis/298269-astropede"/>
+    <hyperlink ref="A61" r:id="rId100" display="https://gamefaqs.gamespot.com/genesis/586035-atomic-robo-kid"/>
+    <hyperlink ref="A62" r:id="rId101" display="https://gamefaqs.gamespot.com/genesis/586036-atomic-runner"/>
+    <hyperlink ref="B62" r:id="rId102" display="https://gamefaqs.gamespot.com/genesis/586036-atomic-runner/cheats"/>
+    <hyperlink ref="A63" r:id="rId103" display="https://gamefaqs.gamespot.com/genesis/586037-atp-tour-championship-tennis"/>
+    <hyperlink ref="B63" r:id="rId104" display="https://gamefaqs.gamespot.com/genesis/586037-atp-tour-championship-tennis/cheats"/>
+    <hyperlink ref="A64" r:id="rId105" display="https://gamefaqs.gamespot.com/genesis/586037-atp-tour-championship-tennis"/>
+    <hyperlink ref="B64" r:id="rId106" display="https://gamefaqs.gamespot.com/genesis/586037-atp-tour-championship-tennis/cheats"/>
+    <hyperlink ref="A65" r:id="rId107" display="https://gamefaqs.gamespot.com/genesis/388525-attack-of-the-petscii-robots"/>
+    <hyperlink ref="A66" r:id="rId108" display="https://gamefaqs.gamespot.com/genesis/581771-australian-rugby-league"/>
+    <hyperlink ref="B66" r:id="rId109" display="https://gamefaqs.gamespot.com/genesis/581771-australian-rugby-league/cheats"/>
+    <hyperlink ref="A67" r:id="rId110" display="https://gamefaqs.gamespot.com/genesis/563313-awesome-possum"/>
+    <hyperlink ref="B67" r:id="rId111" display="https://gamefaqs.gamespot.com/genesis/563313-awesome-possum/cheats"/>
+    <hyperlink ref="A68" r:id="rId112" display="https://gamefaqs.gamespot.com/genesis/951913-aworg"/>
+    <hyperlink ref="A69" r:id="rId113" display="https://gamefaqs.gamespot.com/genesis/563346-ayrton-sennas-super-monaco-gp-ii"/>
+    <hyperlink ref="B69" r:id="rId114" display="https://gamefaqs.gamespot.com/genesis/563346-ayrton-sennas-super-monaco-gp-ii/cheats"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>